<commit_message>
Backup QR Scanner data - 2025-10-14T05:56:44.933Z - Cache Bust: 1760421404933
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Pharmacology_scanner1760420438331_4791e799a156631a1e6528d73ff0b32fbeeb62851b63d680bacede618e9287f5.xlsx
+++ b/log_history/Y2_B2526_Pharmacology_scanner1760420438331_4791e799a156631a1e6528d73ff0b32fbeeb62851b63d680bacede618e9287f5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Pharmacology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -482,9 +482,69 @@
         <v>marian.samir@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>244647</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Pharmacology</v>
+      </c>
+      <c r="C5" t="str">
+        <v>14/10/2025</v>
+      </c>
+      <c r="D5" t="str">
+        <v>08:44:52</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F5" t="str">
+        <v>marian.samir@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>244910</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Pharmacology</v>
+      </c>
+      <c r="C6" t="str">
+        <v>14/10/2025</v>
+      </c>
+      <c r="D6" t="str">
+        <v>08:45:12</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F6" t="str">
+        <v>marian.samir@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>244783</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Pharmacology</v>
+      </c>
+      <c r="C7" t="str">
+        <v>14/10/2025</v>
+      </c>
+      <c r="D7" t="str">
+        <v>08:45:17</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F7" t="str">
+        <v>marian.samir@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>